<commit_message>
interim stable version with pretty output
</commit_message>
<xml_diff>
--- a/positions_with_links.xlsx
+++ b/positions_with_links.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_works\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\parser_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12195" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="46">
   <si>
     <t>Bernina</t>
   </si>
@@ -495,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,4 +1017,57 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1">
+        <v>5990</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>7700</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E1" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
simplified the condition of onliner price existence
</commit_message>
<xml_diff>
--- a/positions_with_links.xlsx
+++ b/positions_with_links.xlsx
@@ -9,13 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12195" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12195" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="Лист4" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="out1_1" localSheetId="3">Лист4!$A$1:$F$21</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,8 +29,25 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="out1" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="D:\Python\parser_python\out1.csv" decimal="," thousands=" " tab="0" comma="1">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="78">
   <si>
     <t>Bernina</t>
   </si>
@@ -164,6 +185,102 @@
   </si>
   <si>
     <t>https://catalog.onliner.by/overlock/bernina/funlockb48</t>
+  </si>
+  <si>
+    <t>manufacturer</t>
+  </si>
+  <si>
+    <t>machine_name</t>
+  </si>
+  <si>
+    <t>onliner_link</t>
+  </si>
+  <si>
+    <t>your_onliner_price</t>
+  </si>
+  <si>
+    <t>their_onliner_price</t>
+  </si>
+  <si>
+    <t>5990,00 р.</t>
+  </si>
+  <si>
+    <t>7700,00 р.</t>
+  </si>
+  <si>
+    <t>5990.0</t>
+  </si>
+  <si>
+    <t>7700.0</t>
+  </si>
+  <si>
+    <t>3600.0</t>
+  </si>
+  <si>
+    <t>3600,00 р.</t>
+  </si>
+  <si>
+    <t>12100.0</t>
+  </si>
+  <si>
+    <t>12 100,00 р.</t>
+  </si>
+  <si>
+    <t>2500.0</t>
+  </si>
+  <si>
+    <t>2300,00 – 2500,00 р.</t>
+  </si>
+  <si>
+    <t>287.0</t>
+  </si>
+  <si>
+    <t>295,00 – 368,87 р.</t>
+  </si>
+  <si>
+    <t>1650.0</t>
+  </si>
+  <si>
+    <t>1650,00 р.</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>Net v nalichii</t>
+  </si>
+  <si>
+    <t>249.0</t>
+  </si>
+  <si>
+    <t>460,00 р.</t>
+  </si>
+  <si>
+    <t>550,00 р.</t>
+  </si>
+  <si>
+    <t>479.9</t>
+  </si>
+  <si>
+    <t>479,90 – 480,26 р.</t>
+  </si>
+  <si>
+    <t>469.9</t>
+  </si>
+  <si>
+    <t>469,90 р.</t>
+  </si>
+  <si>
+    <t>837.0</t>
+  </si>
+  <si>
+    <t>837,00 – 897,00 р.</t>
+  </si>
+  <si>
+    <t>1295.0</t>
+  </si>
+  <si>
+    <t>1295,00 – 1492,50 р.</t>
   </si>
 </sst>
 </file>
@@ -229,6 +346,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="out1_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1023,7 +1144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -1070,4 +1191,442 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>